<commit_message>
Fixed the Ftux.bat + Offer popup now gets triggered after 2 runs instead of 4!
Former-commit-id: 6db072ecc45a5c9bc4d81f75bd78d7b23504edfc
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_FtuxSettings.xlsx
+++ b/Docs/Content/HungryDragonContent_FtuxSettings.xlsx
@@ -986,7 +986,7 @@
   <dimension ref="A1:N5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1090,13 +1090,13 @@
         <v>3</v>
       </c>
       <c r="H5" s="14">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I5" s="14">
         <v>12</v>
       </c>
       <c r="J5" s="14">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="K5" s="14">
         <v>3</v>

</xml_diff>

<commit_message>
Lowered the number of runs required to display the Live Ops popups!
Former-commit-id: 3e25db7ac3a9739deb6e9e25869720179aba5c8d
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_FtuxSettings.xlsx
+++ b/Docs/Content/HungryDragonContent_FtuxSettings.xlsx
@@ -986,7 +986,7 @@
   <dimension ref="A1:N5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1093,7 +1093,7 @@
         <v>4</v>
       </c>
       <c r="I5" s="14">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="J5" s="14">
         <v>2</v>

</xml_diff>

<commit_message>
FTUX: Content - Added new columns to individually control when Passive Events and Happy Hour are allowed.
Former-commit-id: 4a882f40d05a70d9cf0f21d3d87ad0844bee4e5a
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_FtuxSettings.xlsx
+++ b/Docs/Content/HungryDragonContent_FtuxSettings.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10112"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\dragon\client\Docs\Content\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aortin/Documents/UBI/FD/Client_iOS/Docs/Content/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66262415-584F-724B-9637-7FBA6BF4429C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="38400" windowHeight="23535"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="23540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="global_settings" sheetId="2" r:id="rId1"/>
@@ -24,12 +25,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Hadrian Semroud</author>
   </authors>
   <commentList>
-    <comment ref="I4" authorId="0" shapeId="0">
+    <comment ref="I4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -58,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>&lt;Definition&gt;</t>
   </si>
@@ -106,12 +107,18 @@
   </si>
   <si>
     <t>[enableEggsAtRun]</t>
+  </si>
+  <si>
+    <t>[enablePassiveEventsAtRun]</t>
+  </si>
+  <si>
+    <t>[enableHappyHourAtRun]3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -310,7 +317,51 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="17">
+  <dxfs count="19">
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
     <dxf>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
@@ -696,22 +747,24 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="gameSettings" displayName="gameSettings" ref="B4:N5" totalsRowShown="0" headerRowDxfId="16" headerRowBorderDxfId="15" tableBorderDxfId="14" totalsRowBorderDxfId="13">
-  <autoFilter ref="B4:N5"/>
-  <tableColumns count="13">
-    <tableColumn id="1" name="{ftuxSettings}" dataDxfId="12"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="11"/>
-    <tableColumn id="3" name="[enableChestsAtRun]" dataDxfId="10"/>
-    <tableColumn id="4" name="[enableEggsAtRun]" dataDxfId="9"/>
-    <tableColumn id="5" name="[enableMissionsAtRun]" dataDxfId="8"/>
-    <tableColumn id="6" name="[enableQuestsAtRun]" dataDxfId="7"/>
-    <tableColumn id="15" name="[enableTournamentsAtRun]" dataDxfId="6"/>
-    <tableColumn id="16" name="[enableInterstitialPopupsAtRun]" dataDxfId="5"/>
-    <tableColumn id="7" name="[enableOffersPopupAtRun]" dataDxfId="4"/>
-    <tableColumn id="8" name="[enableSharkPetRewardPopupAtRun]" dataDxfId="3"/>
-    <tableColumn id="17" name="[enableLeaguesAtRun]" dataDxfId="2"/>
-    <tableColumn id="9" name="[enableDailyRewardsAtRun]" dataDxfId="1"/>
-    <tableColumn id="10" name="[enableShareButtonsAtRun]" dataDxfId="0"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="gameSettings" displayName="gameSettings" ref="B4:P5" totalsRowShown="0" headerRowDxfId="18" headerRowBorderDxfId="17" tableBorderDxfId="16" totalsRowBorderDxfId="15">
+  <autoFilter ref="B4:P5" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <tableColumns count="15">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="{ftuxSettings}" dataDxfId="14"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="[sku]" dataDxfId="13"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="[enableChestsAtRun]" dataDxfId="12"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="[enableEggsAtRun]" dataDxfId="11"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="[enableMissionsAtRun]" dataDxfId="10"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="[enableQuestsAtRun]" dataDxfId="9"/>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="[enableTournamentsAtRun]" dataDxfId="8"/>
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="[enableInterstitialPopupsAtRun]" dataDxfId="7"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="[enableOffersPopupAtRun]" dataDxfId="6"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="[enableSharkPetRewardPopupAtRun]" dataDxfId="5"/>
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="[enableLeaguesAtRun]" dataDxfId="4"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="[enableDailyRewardsAtRun]" dataDxfId="3"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="[enableShareButtonsAtRun]" dataDxfId="2"/>
+    <tableColumn id="11" xr3:uid="{7C1FA916-A34E-E54F-B557-A82241CCFA1F}" name="[enablePassiveEventsAtRun]" dataDxfId="1"/>
+    <tableColumn id="12" xr3:uid="{3F9ACAE0-12FB-1240-92B4-8D3069A96353}" name="[enableHappyHourAtRun]3" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -979,30 +1032,30 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <tabColor theme="1"/>
   </sheetPr>
-  <dimension ref="A1:N5"/>
+  <dimension ref="A1:P5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+      <selection activeCell="Q5" sqref="Q5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="2.7109375" customWidth="1"/>
-    <col min="2" max="2" width="17.7109375" customWidth="1"/>
-    <col min="3" max="3" width="23.42578125" customWidth="1"/>
-    <col min="4" max="4" width="46.7109375" customWidth="1"/>
+    <col min="1" max="1" width="2.6640625" customWidth="1"/>
+    <col min="2" max="2" width="17.6640625" customWidth="1"/>
+    <col min="3" max="3" width="23.5" customWidth="1"/>
+    <col min="4" max="4" width="46.6640625" customWidth="1"/>
     <col min="5" max="5" width="27" customWidth="1"/>
     <col min="6" max="6" width="31" customWidth="1"/>
-    <col min="7" max="7" width="15.85546875" customWidth="1"/>
+    <col min="7" max="7" width="15.83203125" customWidth="1"/>
     <col min="8" max="22" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="1:14" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:16" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="1:16" ht="24" x14ac:dyDescent="0.3">
       <c r="B2" s="7" t="s">
         <v>2</v>
       </c>
@@ -1016,7 +1069,7 @@
       <c r="J2" s="7"/>
       <c r="K2" s="7"/>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3" s="10"/>
       <c r="B3" s="13"/>
       <c r="C3" s="12"/>
@@ -1029,7 +1082,7 @@
       <c r="J3" s="10"/>
       <c r="K3" s="10"/>
     </row>
-    <row r="4" spans="1:14" ht="174.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" ht="175" x14ac:dyDescent="0.2">
       <c r="B4" s="6" t="s">
         <v>3</v>
       </c>
@@ -1069,8 +1122,14 @@
       <c r="N4" s="9" t="s">
         <v>14</v>
       </c>
+      <c r="O4" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="P4" s="9" t="s">
+        <v>17</v>
+      </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B5" s="3" t="s">
         <v>0</v>
       </c>
@@ -1108,12 +1167,18 @@
         <v>2</v>
       </c>
       <c r="N5" s="14">
+        <v>4</v>
+      </c>
+      <c r="O5" s="14">
+        <v>4</v>
+      </c>
+      <c r="P5" s="14">
         <v>4</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation allowBlank="1" showErrorMessage="1" prompt="percentage [0..1]" sqref="D5:E5"/>
+    <dataValidation allowBlank="1" showErrorMessage="1" prompt="percentage [0..1]" sqref="D5:E5" xr:uid="{00000000-0002-0000-0000-000000000000}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Add UI settings to excel doc
Former-commit-id: 266f2c0b88d10fa8404eb7c25248eadc84291fcd
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_FtuxSettings.xlsx
+++ b/Docs/Content/HungryDragonContent_FtuxSettings.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10112"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10307"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aortin/Documents/UBI/FD/Client_iOS/Docs/Content/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jolea/Projects/client/Docs/Content/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66262415-584F-724B-9637-7FBA6BF4429C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27933FBE-277D-6746-B149-3C1E9378A8A8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="23540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="global_settings" sheetId="2" r:id="rId1"/>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="25">
   <si>
     <t>&lt;Definition&gt;</t>
   </si>
@@ -112,7 +112,28 @@
     <t>[enablePassiveEventsAtRun]</t>
   </si>
   <si>
-    <t>[enableHappyHourAtRun]3</t>
+    <t>UI SETTINGS</t>
+  </si>
+  <si>
+    <t>{UISettings}</t>
+  </si>
+  <si>
+    <t>UISettings</t>
+  </si>
+  <si>
+    <t>[showNextDragonInXpBar]</t>
+  </si>
+  <si>
+    <t>[showUnlockProgressionText]</t>
+  </si>
+  <si>
+    <t>[mapAsButton]</t>
+  </si>
+  <si>
+    <t>[enableHappyHourAtRun]</t>
+  </si>
+  <si>
+    <t>[disableMapParticlesAtRun]</t>
   </si>
 </sst>
 </file>
@@ -171,7 +192,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -208,8 +229,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor theme="4" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="6">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -276,11 +303,37 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -313,11 +366,38 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment textRotation="45"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="19">
+  <dxfs count="20">
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
     <dxf>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
@@ -687,16 +767,16 @@
     </dxf>
     <dxf>
       <border outline="0">
-        <right style="thin">
-          <color auto="1"/>
-        </right>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
       </border>
     </dxf>
     <dxf>
       <border outline="0">
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
       </border>
     </dxf>
     <dxf>
@@ -747,24 +827,25 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="gameSettings" displayName="gameSettings" ref="B4:P5" totalsRowShown="0" headerRowDxfId="18" headerRowBorderDxfId="17" tableBorderDxfId="16" totalsRowBorderDxfId="15">
-  <autoFilter ref="B4:P5" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
-  <tableColumns count="15">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="{ftuxSettings}" dataDxfId="14"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="[sku]" dataDxfId="13"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="[enableChestsAtRun]" dataDxfId="12"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="[enableEggsAtRun]" dataDxfId="11"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="[enableMissionsAtRun]" dataDxfId="10"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="[enableQuestsAtRun]" dataDxfId="9"/>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="[enableTournamentsAtRun]" dataDxfId="8"/>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="[enableInterstitialPopupsAtRun]" dataDxfId="7"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="[enableOffersPopupAtRun]" dataDxfId="6"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="[enableSharkPetRewardPopupAtRun]" dataDxfId="5"/>
-    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="[enableLeaguesAtRun]" dataDxfId="4"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="[enableDailyRewardsAtRun]" dataDxfId="3"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="[enableShareButtonsAtRun]" dataDxfId="2"/>
-    <tableColumn id="11" xr3:uid="{7C1FA916-A34E-E54F-B557-A82241CCFA1F}" name="[enablePassiveEventsAtRun]" dataDxfId="1"/>
-    <tableColumn id="12" xr3:uid="{3F9ACAE0-12FB-1240-92B4-8D3069A96353}" name="[enableHappyHourAtRun]3" dataDxfId="0"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="gameSettings" displayName="gameSettings" ref="B4:Q5" totalsRowShown="0" headerRowDxfId="19" headerRowBorderDxfId="17" tableBorderDxfId="18" totalsRowBorderDxfId="16">
+  <autoFilter ref="B4:Q5" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <tableColumns count="16">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="{ftuxSettings}" dataDxfId="15"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="[sku]" dataDxfId="14"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="[enableChestsAtRun]" dataDxfId="13"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="[enableEggsAtRun]" dataDxfId="12"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="[enableMissionsAtRun]" dataDxfId="11"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="[enableQuestsAtRun]" dataDxfId="10"/>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="[enableTournamentsAtRun]" dataDxfId="9"/>
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="[enableInterstitialPopupsAtRun]" dataDxfId="8"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="[enableOffersPopupAtRun]" dataDxfId="7"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="[enableSharkPetRewardPopupAtRun]" dataDxfId="6"/>
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="[enableLeaguesAtRun]" dataDxfId="5"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="[enableDailyRewardsAtRun]" dataDxfId="4"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="[enableShareButtonsAtRun]" dataDxfId="3"/>
+    <tableColumn id="11" xr3:uid="{7C1FA916-A34E-E54F-B557-A82241CCFA1F}" name="[enablePassiveEventsAtRun]" dataDxfId="2"/>
+    <tableColumn id="12" xr3:uid="{3F9ACAE0-12FB-1240-92B4-8D3069A96353}" name="[enableHappyHourAtRun]" dataDxfId="1"/>
+    <tableColumn id="13" xr3:uid="{36EFFF74-0DB8-FF49-8108-D6E88C4ACBB5}" name="[disableMapParticlesAtRun]" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1036,10 +1117,10 @@
   <sheetPr>
     <tabColor theme="1"/>
   </sheetPr>
-  <dimension ref="A1:P5"/>
+  <dimension ref="A1:Q11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Q5" sqref="Q5"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1054,8 +1135,8 @@
     <col min="8" max="22" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="1:16" ht="24" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="1:17" ht="24" x14ac:dyDescent="0.3">
       <c r="B2" s="7" t="s">
         <v>2</v>
       </c>
@@ -1069,7 +1150,7 @@
       <c r="J2" s="7"/>
       <c r="K2" s="7"/>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A3" s="10"/>
       <c r="B3" s="13"/>
       <c r="C3" s="12"/>
@@ -1082,7 +1163,7 @@
       <c r="J3" s="10"/>
       <c r="K3" s="10"/>
     </row>
-    <row r="4" spans="1:16" ht="175" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:17" ht="175" x14ac:dyDescent="0.2">
       <c r="B4" s="6" t="s">
         <v>3</v>
       </c>
@@ -1126,10 +1207,13 @@
         <v>16</v>
       </c>
       <c r="P4" s="9" t="s">
-        <v>17</v>
+        <v>23</v>
+      </c>
+      <c r="Q4" s="4" t="s">
+        <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B5" s="3" t="s">
         <v>0</v>
       </c>
@@ -1174,11 +1258,73 @@
       </c>
       <c r="P5" s="14">
         <v>4</v>
+      </c>
+      <c r="Q5" s="18">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="8" spans="1:17" ht="24" x14ac:dyDescent="0.3">
+      <c r="B8" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="7"/>
+      <c r="H8" s="7"/>
+      <c r="I8" s="7"/>
+      <c r="J8" s="7"/>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="B9" s="13"/>
+      <c r="C9" s="12"/>
+      <c r="D9" s="11"/>
+      <c r="E9" s="12"/>
+      <c r="F9" s="12"/>
+      <c r="G9" s="12"/>
+      <c r="H9" s="12"/>
+      <c r="I9" s="11"/>
+      <c r="J9" s="10"/>
+    </row>
+    <row r="10" spans="1:17" ht="142" x14ac:dyDescent="0.2">
+      <c r="B10" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D10" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="E10" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="F10" s="17" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="B11" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D11" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="E11" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="F11" s="16" t="b">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation allowBlank="1" showErrorMessage="1" prompt="percentage [0..1]" sqref="D5:E5" xr:uid="{00000000-0002-0000-0000-000000000000}"/>
+    <dataValidation allowBlank="1" showErrorMessage="1" prompt="percentage [0..1]" sqref="D5:E5 D11:E11" xr:uid="{00000000-0002-0000-0000-000000000000}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
In game - Make a variation of the map button for AB test
Former-commit-id: 255609d7b1270ff5745243dbdf1bc52bed706242
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_FtuxSettings.xlsx
+++ b/Docs/Content/HungryDragonContent_FtuxSettings.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jolea/Projects/client/Docs/Content/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27933FBE-277D-6746-B149-3C1E9378A8A8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81D6AB18-222F-1947-89F6-E33CE800451A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -767,16 +767,16 @@
     </dxf>
     <dxf>
       <border outline="0">
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
       </border>
     </dxf>
     <dxf>
       <border outline="0">
-        <right style="thin">
-          <color auto="1"/>
-        </right>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
       </border>
     </dxf>
     <dxf>
@@ -827,7 +827,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="gameSettings" displayName="gameSettings" ref="B4:Q5" totalsRowShown="0" headerRowDxfId="19" headerRowBorderDxfId="17" tableBorderDxfId="18" totalsRowBorderDxfId="16">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="gameSettings" displayName="gameSettings" ref="B4:Q5" totalsRowShown="0" headerRowDxfId="19" headerRowBorderDxfId="18" tableBorderDxfId="17" totalsRowBorderDxfId="16">
   <autoFilter ref="B4:Q5" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="16">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="{ftuxSettings}" dataDxfId="15"/>
@@ -1120,7 +1120,7 @@
   <dimension ref="A1:Q11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="T4" sqref="T4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
In Game - Create two variants of the map button layout for AB testing
Former-commit-id: 863486bfaf7f6284d348fb79ef16c8e5e8740ba0
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_FtuxSettings.xlsx
+++ b/Docs/Content/HungryDragonContent_FtuxSettings.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jolea/Projects/client/Docs/Content/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81D6AB18-222F-1947-89F6-E33CE800451A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4ACE8555-F423-1A4A-B244-311FE1279E17}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="global_settings" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="26">
   <si>
     <t>&lt;Definition&gt;</t>
   </si>
@@ -134,13 +134,16 @@
   </si>
   <si>
     <t>[disableMapParticlesAtRun]</t>
+  </si>
+  <si>
+    <t>[enableMapAtRun]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -190,6 +193,12 @@
       <color indexed="81"/>
       <name val="Tahoma"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="8">
@@ -333,7 +342,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -371,11 +380,32 @@
       <alignment textRotation="45"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment textRotation="45"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="20">
+  <dxfs count="21">
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
     <dxf>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
@@ -827,25 +857,26 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="gameSettings" displayName="gameSettings" ref="B4:Q5" totalsRowShown="0" headerRowDxfId="19" headerRowBorderDxfId="18" tableBorderDxfId="17" totalsRowBorderDxfId="16">
-  <autoFilter ref="B4:Q5" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
-  <tableColumns count="16">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="{ftuxSettings}" dataDxfId="15"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="[sku]" dataDxfId="14"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="[enableChestsAtRun]" dataDxfId="13"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="[enableEggsAtRun]" dataDxfId="12"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="[enableMissionsAtRun]" dataDxfId="11"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="[enableQuestsAtRun]" dataDxfId="10"/>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="[enableTournamentsAtRun]" dataDxfId="9"/>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="[enableInterstitialPopupsAtRun]" dataDxfId="8"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="[enableOffersPopupAtRun]" dataDxfId="7"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="[enableSharkPetRewardPopupAtRun]" dataDxfId="6"/>
-    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="[enableLeaguesAtRun]" dataDxfId="5"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="[enableDailyRewardsAtRun]" dataDxfId="4"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="[enableShareButtonsAtRun]" dataDxfId="3"/>
-    <tableColumn id="11" xr3:uid="{7C1FA916-A34E-E54F-B557-A82241CCFA1F}" name="[enablePassiveEventsAtRun]" dataDxfId="2"/>
-    <tableColumn id="12" xr3:uid="{3F9ACAE0-12FB-1240-92B4-8D3069A96353}" name="[enableHappyHourAtRun]" dataDxfId="1"/>
-    <tableColumn id="13" xr3:uid="{36EFFF74-0DB8-FF49-8108-D6E88C4ACBB5}" name="[disableMapParticlesAtRun]" dataDxfId="0"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="gameSettings" displayName="gameSettings" ref="B4:R5" totalsRowShown="0" headerRowDxfId="20" headerRowBorderDxfId="19" tableBorderDxfId="18" totalsRowBorderDxfId="17">
+  <autoFilter ref="B4:R5" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <tableColumns count="17">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="{ftuxSettings}" dataDxfId="16"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="[sku]" dataDxfId="15"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="[enableChestsAtRun]" dataDxfId="14"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="[enableEggsAtRun]" dataDxfId="13"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="[enableMissionsAtRun]" dataDxfId="12"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="[enableQuestsAtRun]" dataDxfId="11"/>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="[enableTournamentsAtRun]" dataDxfId="10"/>
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="[enableInterstitialPopupsAtRun]" dataDxfId="9"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="[enableOffersPopupAtRun]" dataDxfId="8"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="[enableSharkPetRewardPopupAtRun]" dataDxfId="7"/>
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="[enableLeaguesAtRun]" dataDxfId="6"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="[enableDailyRewardsAtRun]" dataDxfId="5"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="[enableShareButtonsAtRun]" dataDxfId="4"/>
+    <tableColumn id="11" xr3:uid="{7C1FA916-A34E-E54F-B557-A82241CCFA1F}" name="[enablePassiveEventsAtRun]" dataDxfId="3"/>
+    <tableColumn id="12" xr3:uid="{3F9ACAE0-12FB-1240-92B4-8D3069A96353}" name="[enableHappyHourAtRun]" dataDxfId="2"/>
+    <tableColumn id="13" xr3:uid="{36EFFF74-0DB8-FF49-8108-D6E88C4ACBB5}" name="[enableMapAtRun]" dataDxfId="0"/>
+    <tableColumn id="14" xr3:uid="{D1ADB192-6387-3F4C-9C6F-BF33BBC8F7F6}" name="[disableMapParticlesAtRun]" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1117,10 +1148,10 @@
   <sheetPr>
     <tabColor theme="1"/>
   </sheetPr>
-  <dimension ref="A1:Q11"/>
+  <dimension ref="A1:R11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="T4" sqref="T4"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="R5" sqref="R5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1135,8 +1166,8 @@
     <col min="8" max="22" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="1:17" ht="24" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="1:18" ht="24" x14ac:dyDescent="0.3">
       <c r="B2" s="7" t="s">
         <v>2</v>
       </c>
@@ -1150,7 +1181,7 @@
       <c r="J2" s="7"/>
       <c r="K2" s="7"/>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A3" s="10"/>
       <c r="B3" s="13"/>
       <c r="C3" s="12"/>
@@ -1163,7 +1194,7 @@
       <c r="J3" s="10"/>
       <c r="K3" s="10"/>
     </row>
-    <row r="4" spans="1:17" ht="175" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:18" ht="175" x14ac:dyDescent="0.2">
       <c r="B4" s="6" t="s">
         <v>3</v>
       </c>
@@ -1209,11 +1240,14 @@
       <c r="P4" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="Q4" s="4" t="s">
+      <c r="Q4" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="R4" s="19" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B5" s="3" t="s">
         <v>0</v>
       </c>
@@ -1259,12 +1293,15 @@
       <c r="P5" s="14">
         <v>4</v>
       </c>
-      <c r="Q5" s="18">
+      <c r="Q5" s="14">
+        <v>1</v>
+      </c>
+      <c r="R5" s="18">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:17" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="8" spans="1:17" ht="24" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:18" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="8" spans="1:18" ht="24" x14ac:dyDescent="0.3">
       <c r="B8" s="7" t="s">
         <v>17</v>
       </c>
@@ -1277,7 +1314,7 @@
       <c r="I8" s="7"/>
       <c r="J8" s="7"/>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B9" s="13"/>
       <c r="C9" s="12"/>
       <c r="D9" s="11"/>
@@ -1288,7 +1325,7 @@
       <c r="I9" s="11"/>
       <c r="J9" s="10"/>
     </row>
-    <row r="10" spans="1:17" ht="142" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:18" ht="142" x14ac:dyDescent="0.2">
       <c r="B10" s="6" t="s">
         <v>18</v>
       </c>
@@ -1305,7 +1342,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B11" s="3" t="s">
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
FALSE all th FTUEX ab test options
Former-commit-id: 7bb11e676410065022456d902d09cd7da5155d73
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_FtuxSettings.xlsx
+++ b/Docs/Content/HungryDragonContent_FtuxSettings.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10307"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jolea/Projects/client/Docs/Content/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\dragon\client\Docs\Content\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4ACE8555-F423-1A4A-B244-311FE1279E17}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="28800" windowHeight="15945"/>
   </bookViews>
   <sheets>
     <sheet name="global_settings" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,12 +24,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Hadrian Semroud</author>
   </authors>
   <commentList>
-    <comment ref="I4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
+    <comment ref="I4" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -142,7 +141,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -391,6 +390,28 @@
     <dxf>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
           <color auto="1"/>
         </left>
         <right style="thin">
@@ -404,28 +425,6 @@
         </bottom>
         <vertical/>
         <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
       </border>
     </dxf>
     <dxf>
@@ -857,26 +856,26 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="gameSettings" displayName="gameSettings" ref="B4:R5" totalsRowShown="0" headerRowDxfId="20" headerRowBorderDxfId="19" tableBorderDxfId="18" totalsRowBorderDxfId="17">
-  <autoFilter ref="B4:R5" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="gameSettings" displayName="gameSettings" ref="B4:R5" totalsRowShown="0" headerRowDxfId="20" headerRowBorderDxfId="19" tableBorderDxfId="18" totalsRowBorderDxfId="17">
+  <autoFilter ref="B4:R5"/>
   <tableColumns count="17">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="{ftuxSettings}" dataDxfId="16"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="[sku]" dataDxfId="15"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="[enableChestsAtRun]" dataDxfId="14"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="[enableEggsAtRun]" dataDxfId="13"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="[enableMissionsAtRun]" dataDxfId="12"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="[enableQuestsAtRun]" dataDxfId="11"/>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="[enableTournamentsAtRun]" dataDxfId="10"/>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="[enableInterstitialPopupsAtRun]" dataDxfId="9"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="[enableOffersPopupAtRun]" dataDxfId="8"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="[enableSharkPetRewardPopupAtRun]" dataDxfId="7"/>
-    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="[enableLeaguesAtRun]" dataDxfId="6"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="[enableDailyRewardsAtRun]" dataDxfId="5"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="[enableShareButtonsAtRun]" dataDxfId="4"/>
-    <tableColumn id="11" xr3:uid="{7C1FA916-A34E-E54F-B557-A82241CCFA1F}" name="[enablePassiveEventsAtRun]" dataDxfId="3"/>
-    <tableColumn id="12" xr3:uid="{3F9ACAE0-12FB-1240-92B4-8D3069A96353}" name="[enableHappyHourAtRun]" dataDxfId="2"/>
-    <tableColumn id="13" xr3:uid="{36EFFF74-0DB8-FF49-8108-D6E88C4ACBB5}" name="[enableMapAtRun]" dataDxfId="0"/>
-    <tableColumn id="14" xr3:uid="{D1ADB192-6387-3F4C-9C6F-BF33BBC8F7F6}" name="[disableMapParticlesAtRun]" dataDxfId="1"/>
+    <tableColumn id="1" name="{ftuxSettings}" dataDxfId="16"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="15"/>
+    <tableColumn id="3" name="[enableChestsAtRun]" dataDxfId="14"/>
+    <tableColumn id="4" name="[enableEggsAtRun]" dataDxfId="13"/>
+    <tableColumn id="5" name="[enableMissionsAtRun]" dataDxfId="12"/>
+    <tableColumn id="6" name="[enableQuestsAtRun]" dataDxfId="11"/>
+    <tableColumn id="15" name="[enableTournamentsAtRun]" dataDxfId="10"/>
+    <tableColumn id="16" name="[enableInterstitialPopupsAtRun]" dataDxfId="9"/>
+    <tableColumn id="7" name="[enableOffersPopupAtRun]" dataDxfId="8"/>
+    <tableColumn id="8" name="[enableSharkPetRewardPopupAtRun]" dataDxfId="7"/>
+    <tableColumn id="17" name="[enableLeaguesAtRun]" dataDxfId="6"/>
+    <tableColumn id="9" name="[enableDailyRewardsAtRun]" dataDxfId="5"/>
+    <tableColumn id="10" name="[enableShareButtonsAtRun]" dataDxfId="4"/>
+    <tableColumn id="11" name="[enablePassiveEventsAtRun]" dataDxfId="3"/>
+    <tableColumn id="12" name="[enableHappyHourAtRun]" dataDxfId="2"/>
+    <tableColumn id="13" name="[enableMapAtRun]" dataDxfId="1"/>
+    <tableColumn id="14" name="[disableMapParticlesAtRun]" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1144,30 +1143,30 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="1"/>
   </sheetPr>
   <dimension ref="A1:R11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="R5" sqref="R5"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.6640625" customWidth="1"/>
-    <col min="2" max="2" width="17.6640625" customWidth="1"/>
-    <col min="3" max="3" width="23.5" customWidth="1"/>
-    <col min="4" max="4" width="46.6640625" customWidth="1"/>
+    <col min="1" max="1" width="2.7109375" customWidth="1"/>
+    <col min="2" max="2" width="17.7109375" customWidth="1"/>
+    <col min="3" max="3" width="23.42578125" customWidth="1"/>
+    <col min="4" max="4" width="46.7109375" customWidth="1"/>
     <col min="5" max="5" width="27" customWidth="1"/>
     <col min="6" max="6" width="31" customWidth="1"/>
-    <col min="7" max="7" width="15.83203125" customWidth="1"/>
+    <col min="7" max="7" width="15.85546875" customWidth="1"/>
     <col min="8" max="22" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="1:18" ht="24" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:18" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B2" s="7" t="s">
         <v>2</v>
       </c>
@@ -1181,7 +1180,7 @@
       <c r="J2" s="7"/>
       <c r="K2" s="7"/>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="10"/>
       <c r="B3" s="13"/>
       <c r="C3" s="12"/>
@@ -1194,7 +1193,7 @@
       <c r="J3" s="10"/>
       <c r="K3" s="10"/>
     </row>
-    <row r="4" spans="1:18" ht="175" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:18" ht="174.75" x14ac:dyDescent="0.25">
       <c r="B4" s="6" t="s">
         <v>3</v>
       </c>
@@ -1247,7 +1246,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
         <v>0</v>
       </c>
@@ -1300,8 +1299,8 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:18" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="8" spans="1:18" ht="24" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="8" spans="1:18" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B8" s="7" t="s">
         <v>17</v>
       </c>
@@ -1314,7 +1313,7 @@
       <c r="I8" s="7"/>
       <c r="J8" s="7"/>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B9" s="13"/>
       <c r="C9" s="12"/>
       <c r="D9" s="11"/>
@@ -1325,7 +1324,7 @@
       <c r="I9" s="11"/>
       <c r="J9" s="10"/>
     </row>
-    <row r="10" spans="1:18" ht="142" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:18" ht="142.5" x14ac:dyDescent="0.25">
       <c r="B10" s="6" t="s">
         <v>18</v>
       </c>
@@ -1342,7 +1341,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B11" s="3" t="s">
         <v>0</v>
       </c>
@@ -1350,18 +1349,18 @@
         <v>19</v>
       </c>
       <c r="D11" s="16" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E11" s="16" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F11" s="16" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation allowBlank="1" showErrorMessage="1" prompt="percentage [0..1]" sqref="D5:E5 D11:E11" xr:uid="{00000000-0002-0000-0000-000000000000}"/>
+    <dataValidation allowBlank="1" showErrorMessage="1" prompt="percentage [0..1]" sqref="D5:E5 D11:E11"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
FTUX Settings: Content - Added new flag "enableDragonDiscountsAtRun".
Former-commit-id: baf6fd4894afc736776c0a14ab26f7bbd5e2c0fb
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_FtuxSettings.xlsx
+++ b/Docs/Content/HungryDragonContent_FtuxSettings.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\dragon\client\Docs\Content\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Ubi\HungryDragon\HD_Client\Docs\Content\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96129193-78F3-446D-89CA-DAA0E2741552}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="28800" windowHeight="15945"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21090" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="global_settings" sheetId="2" r:id="rId1"/>
@@ -24,12 +25,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Hadrian Semroud</author>
   </authors>
   <commentList>
-    <comment ref="I4" authorId="0" shapeId="0">
+    <comment ref="I4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -58,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="27">
   <si>
     <t>&lt;Definition&gt;</t>
   </si>
@@ -136,12 +137,15 @@
   </si>
   <si>
     <t>[enableMapAtRun]</t>
+  </si>
+  <si>
+    <t>[enableDragonDiscountsAtRun]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -244,7 +248,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -326,22 +330,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -378,7 +371,6 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment textRotation="45"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment textRotation="45"/>
     </xf>
@@ -386,27 +378,41 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="21">
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
+  <dxfs count="22">
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -856,26 +862,27 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="gameSettings" displayName="gameSettings" ref="B4:R5" totalsRowShown="0" headerRowDxfId="20" headerRowBorderDxfId="19" tableBorderDxfId="18" totalsRowBorderDxfId="17">
-  <autoFilter ref="B4:R5"/>
-  <tableColumns count="17">
-    <tableColumn id="1" name="{ftuxSettings}" dataDxfId="16"/>
-    <tableColumn id="2" name="[sku]" dataDxfId="15"/>
-    <tableColumn id="3" name="[enableChestsAtRun]" dataDxfId="14"/>
-    <tableColumn id="4" name="[enableEggsAtRun]" dataDxfId="13"/>
-    <tableColumn id="5" name="[enableMissionsAtRun]" dataDxfId="12"/>
-    <tableColumn id="6" name="[enableQuestsAtRun]" dataDxfId="11"/>
-    <tableColumn id="15" name="[enableTournamentsAtRun]" dataDxfId="10"/>
-    <tableColumn id="16" name="[enableInterstitialPopupsAtRun]" dataDxfId="9"/>
-    <tableColumn id="7" name="[enableOffersPopupAtRun]" dataDxfId="8"/>
-    <tableColumn id="8" name="[enableSharkPetRewardPopupAtRun]" dataDxfId="7"/>
-    <tableColumn id="17" name="[enableLeaguesAtRun]" dataDxfId="6"/>
-    <tableColumn id="9" name="[enableDailyRewardsAtRun]" dataDxfId="5"/>
-    <tableColumn id="10" name="[enableShareButtonsAtRun]" dataDxfId="4"/>
-    <tableColumn id="11" name="[enablePassiveEventsAtRun]" dataDxfId="3"/>
-    <tableColumn id="12" name="[enableHappyHourAtRun]" dataDxfId="2"/>
-    <tableColumn id="13" name="[enableMapAtRun]" dataDxfId="1"/>
-    <tableColumn id="14" name="[disableMapParticlesAtRun]" dataDxfId="0"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="gameSettings" displayName="gameSettings" ref="B4:S5" totalsRowShown="0" headerRowDxfId="21" headerRowBorderDxfId="20" tableBorderDxfId="19" totalsRowBorderDxfId="18">
+  <autoFilter ref="B4:S5" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <tableColumns count="18">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="{ftuxSettings}" dataDxfId="17"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="[sku]" dataDxfId="16"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="[enableChestsAtRun]" dataDxfId="15"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="[enableEggsAtRun]" dataDxfId="14"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="[enableMissionsAtRun]" dataDxfId="13"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="[enableQuestsAtRun]" dataDxfId="12"/>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="[enableTournamentsAtRun]" dataDxfId="11"/>
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="[enableInterstitialPopupsAtRun]" dataDxfId="10"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="[enableOffersPopupAtRun]" dataDxfId="9"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="[enableSharkPetRewardPopupAtRun]" dataDxfId="8"/>
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="[enableLeaguesAtRun]" dataDxfId="7"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="[enableDailyRewardsAtRun]" dataDxfId="6"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="[enableShareButtonsAtRun]" dataDxfId="5"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="[enablePassiveEventsAtRun]" dataDxfId="4"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="[enableHappyHourAtRun]" dataDxfId="3"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="[enableMapAtRun]" dataDxfId="2"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="[disableMapParticlesAtRun]" dataDxfId="1"/>
+    <tableColumn id="18" xr3:uid="{6C0A0519-6FB8-43B2-B252-FEB2849E2839}" name="[enableDragonDiscountsAtRun]" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1143,14 +1150,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <tabColor theme="1"/>
   </sheetPr>
-  <dimension ref="A1:R11"/>
+  <dimension ref="A1:S11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="S9" sqref="S9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1165,8 +1172,8 @@
     <col min="8" max="22" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="1:18" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:19" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B2" s="7" t="s">
         <v>2</v>
       </c>
@@ -1180,7 +1187,7 @@
       <c r="J2" s="7"/>
       <c r="K2" s="7"/>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" s="10"/>
       <c r="B3" s="13"/>
       <c r="C3" s="12"/>
@@ -1193,7 +1200,7 @@
       <c r="J3" s="10"/>
       <c r="K3" s="10"/>
     </row>
-    <row r="4" spans="1:18" ht="174.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" ht="174.75" x14ac:dyDescent="0.25">
       <c r="B4" s="6" t="s">
         <v>3</v>
       </c>
@@ -1242,11 +1249,14 @@
       <c r="Q4" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="R4" s="19" t="s">
+      <c r="R4" s="18" t="s">
         <v>24</v>
       </c>
+      <c r="S4" s="4" t="s">
+        <v>26</v>
+      </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
         <v>0</v>
       </c>
@@ -1295,12 +1305,15 @@
       <c r="Q5" s="14">
         <v>1</v>
       </c>
-      <c r="R5" s="18">
+      <c r="R5" s="14">
         <v>3</v>
       </c>
+      <c r="S5" s="14">
+        <v>4</v>
+      </c>
     </row>
-    <row r="7" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="8" spans="1:18" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="8" spans="1:19" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B8" s="7" t="s">
         <v>17</v>
       </c>
@@ -1313,7 +1326,7 @@
       <c r="I8" s="7"/>
       <c r="J8" s="7"/>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B9" s="13"/>
       <c r="C9" s="12"/>
       <c r="D9" s="11"/>
@@ -1324,7 +1337,7 @@
       <c r="I9" s="11"/>
       <c r="J9" s="10"/>
     </row>
-    <row r="10" spans="1:18" ht="142.5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:19" ht="142.5" x14ac:dyDescent="0.25">
       <c r="B10" s="6" t="s">
         <v>18</v>
       </c>
@@ -1341,7 +1354,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B11" s="3" t="s">
         <v>0</v>
       </c>
@@ -1360,7 +1373,7 @@
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation allowBlank="1" showErrorMessage="1" prompt="percentage [0..1]" sqref="D5:E5 D11:E11"/>
+    <dataValidation allowBlank="1" showErrorMessage="1" prompt="percentage [0..1]" sqref="D5:E5 D11:E11" xr:uid="{00000000-0002-0000-0000-000000000000}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
change naming mods halloween added some new ftuex test to xml
Former-commit-id: 714eca25f6179dbe705f4f349889830ed3d314cc
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_FtuxSettings.xlsx
+++ b/Docs/Content/HungryDragonContent_FtuxSettings.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Ubi\HungryDragon\HD_Client\Docs\Content\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\dragon\client\Docs\Content\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96129193-78F3-446D-89CA-DAA0E2741552}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21090" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21090"/>
   </bookViews>
   <sheets>
     <sheet name="global_settings" sheetId="2" r:id="rId1"/>
@@ -25,12 +24,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Hadrian Semroud</author>
   </authors>
   <commentList>
-    <comment ref="I4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
+    <comment ref="I4" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -59,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="30">
   <si>
     <t>&lt;Definition&gt;</t>
   </si>
@@ -140,12 +139,21 @@
   </si>
   <si>
     <t>[enableDragonDiscountsAtRun]</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> unlockedSkinPowerAsInfoBox</t>
+  </si>
+  <si>
+    <t>showContinueButtonInUnlockedSkin</t>
+  </si>
+  <si>
+    <t>initialMapCountdownTriggeredByPlayer</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -862,27 +870,27 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="gameSettings" displayName="gameSettings" ref="B4:S5" totalsRowShown="0" headerRowDxfId="21" headerRowBorderDxfId="20" tableBorderDxfId="19" totalsRowBorderDxfId="18">
-  <autoFilter ref="B4:S5" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="gameSettings" displayName="gameSettings" ref="B4:S5" totalsRowShown="0" headerRowDxfId="21" headerRowBorderDxfId="20" tableBorderDxfId="19" totalsRowBorderDxfId="18">
+  <autoFilter ref="B4:S5"/>
   <tableColumns count="18">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="{ftuxSettings}" dataDxfId="17"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="[sku]" dataDxfId="16"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="[enableChestsAtRun]" dataDxfId="15"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="[enableEggsAtRun]" dataDxfId="14"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="[enableMissionsAtRun]" dataDxfId="13"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="[enableQuestsAtRun]" dataDxfId="12"/>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="[enableTournamentsAtRun]" dataDxfId="11"/>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="[enableInterstitialPopupsAtRun]" dataDxfId="10"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="[enableOffersPopupAtRun]" dataDxfId="9"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="[enableSharkPetRewardPopupAtRun]" dataDxfId="8"/>
-    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="[enableLeaguesAtRun]" dataDxfId="7"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="[enableDailyRewardsAtRun]" dataDxfId="6"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="[enableShareButtonsAtRun]" dataDxfId="5"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="[enablePassiveEventsAtRun]" dataDxfId="4"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="[enableHappyHourAtRun]" dataDxfId="3"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="[enableMapAtRun]" dataDxfId="2"/>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="[disableMapParticlesAtRun]" dataDxfId="1"/>
-    <tableColumn id="18" xr3:uid="{6C0A0519-6FB8-43B2-B252-FEB2849E2839}" name="[enableDragonDiscountsAtRun]" dataDxfId="0"/>
+    <tableColumn id="1" name="{ftuxSettings}" dataDxfId="17"/>
+    <tableColumn id="2" name="[sku]" dataDxfId="16"/>
+    <tableColumn id="3" name="[enableChestsAtRun]" dataDxfId="15"/>
+    <tableColumn id="4" name="[enableEggsAtRun]" dataDxfId="14"/>
+    <tableColumn id="5" name="[enableMissionsAtRun]" dataDxfId="13"/>
+    <tableColumn id="6" name="[enableQuestsAtRun]" dataDxfId="12"/>
+    <tableColumn id="15" name="[enableTournamentsAtRun]" dataDxfId="11"/>
+    <tableColumn id="16" name="[enableInterstitialPopupsAtRun]" dataDxfId="10"/>
+    <tableColumn id="7" name="[enableOffersPopupAtRun]" dataDxfId="9"/>
+    <tableColumn id="8" name="[enableSharkPetRewardPopupAtRun]" dataDxfId="8"/>
+    <tableColumn id="17" name="[enableLeaguesAtRun]" dataDxfId="7"/>
+    <tableColumn id="9" name="[enableDailyRewardsAtRun]" dataDxfId="6"/>
+    <tableColumn id="10" name="[enableShareButtonsAtRun]" dataDxfId="5"/>
+    <tableColumn id="11" name="[enablePassiveEventsAtRun]" dataDxfId="4"/>
+    <tableColumn id="12" name="[enableHappyHourAtRun]" dataDxfId="3"/>
+    <tableColumn id="13" name="[enableMapAtRun]" dataDxfId="2"/>
+    <tableColumn id="14" name="[disableMapParticlesAtRun]" dataDxfId="1"/>
+    <tableColumn id="18" name="[enableDragonDiscountsAtRun]" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1150,14 +1158,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="1"/>
   </sheetPr>
   <dimension ref="A1:S11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="S9" sqref="S9"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11:I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1337,7 +1345,7 @@
       <c r="I9" s="11"/>
       <c r="J9" s="10"/>
     </row>
-    <row r="10" spans="1:19" ht="142.5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:19" ht="186" x14ac:dyDescent="0.25">
       <c r="B10" s="6" t="s">
         <v>18</v>
       </c>
@@ -1352,6 +1360,15 @@
       </c>
       <c r="F10" s="17" t="s">
         <v>22</v>
+      </c>
+      <c r="G10" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="H10" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="I10" s="17" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
@@ -1370,10 +1387,19 @@
       <c r="F11" s="16" t="b">
         <v>0</v>
       </c>
+      <c r="G11" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="H11" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="I11" s="16" t="b">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation allowBlank="1" showErrorMessage="1" prompt="percentage [0..1]" sqref="D5:E5 D11:E11" xr:uid="{00000000-0002-0000-0000-000000000000}"/>
+    <dataValidation allowBlank="1" showErrorMessage="1" prompt="percentage [0..1]" sqref="D5:E5 D11:E11"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
ftux test if its commiting right
Former-commit-id: 7a49383d13d3b0793d5dcf8b254d16d63a871fb0
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_FtuxSettings.xlsx
+++ b/Docs/Content/HungryDragonContent_FtuxSettings.xlsx
@@ -141,13 +141,13 @@
     <t>[enableDragonDiscountsAtRun]</t>
   </si>
   <si>
-    <t xml:space="preserve"> unlockedSkinPowerAsInfoBox</t>
-  </si>
-  <si>
-    <t>showContinueButtonInUnlockedSkin</t>
-  </si>
-  <si>
-    <t>initialMapCountdownTriggeredByPlayer</t>
+    <t xml:space="preserve"> [unlockedSkinPowerAsInfoBox]</t>
+  </si>
+  <si>
+    <t>[showContinueButtonInUnlockedSkin]</t>
+  </si>
+  <si>
+    <t>[initialMapCountdownTriggeredByPlayer]</t>
   </si>
 </sst>
 </file>
@@ -1333,6 +1333,8 @@
       <c r="H8" s="7"/>
       <c r="I8" s="7"/>
       <c r="J8" s="7"/>
+      <c r="K8" s="7"/>
+      <c r="L8" s="7"/>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B9" s="13"/>
@@ -1345,7 +1347,7 @@
       <c r="I9" s="11"/>
       <c r="J9" s="10"/>
     </row>
-    <row r="10" spans="1:19" ht="186" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:19" ht="192.75" x14ac:dyDescent="0.25">
       <c r="B10" s="6" t="s">
         <v>18</v>
       </c>

</xml_diff>

<commit_message>
enabled these FTUX: map as button next dragon in xp bar unlock progression text
Former-commit-id: d0dcb86b768178d1610ecfd178817dbdac7018f6
</commit_message>
<xml_diff>
--- a/Docs/Content/HungryDragonContent_FtuxSettings.xlsx
+++ b/Docs/Content/HungryDragonContent_FtuxSettings.xlsx
@@ -1165,7 +1165,7 @@
   <dimension ref="A1:S11"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11:I11"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1381,13 +1381,13 @@
         <v>19</v>
       </c>
       <c r="D11" s="16" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E11" s="16" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F11" s="16" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G11" s="16" t="b">
         <v>0</v>

</xml_diff>